<commit_message>
Actualización de plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1319 - CCON,CNOM, Jeniffer Venegas _MO/Planeación/Plan_de_proyecto.xlsx
+++ b/Proyectos/2015/11/P1319 - CCON,CNOM, Jeniffer Venegas _MO/Planeación/Plan_de_proyecto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-60" windowWidth="16380" windowHeight="8250" tabRatio="875" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-60" windowWidth="16380" windowHeight="8250" tabRatio="875"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="160">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -559,12 +559,165 @@
   <si>
     <t>validar implementación</t>
   </si>
+  <si>
+    <t>33 14 21 95 20</t>
+  </si>
+  <si>
+    <t>Francisco Llamas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33 16 36 73 65</t>
+  </si>
+  <si>
+    <t>Jose Francisco Llamas Díaz</t>
+  </si>
+  <si>
+    <t>33 13 32 75 63</t>
+  </si>
+  <si>
+    <t>marisol.ornelas@sos-soft.com</t>
+  </si>
+  <si>
+    <t>oriana.campos@sos-soft.com</t>
+  </si>
+  <si>
+    <t>francisco.llamas@sos-soft.com</t>
+  </si>
+  <si>
+    <t>adriana.jaramillo@sos-soft.com</t>
+  </si>
+  <si>
+    <t>r.novela@sos-soft.com</t>
+  </si>
+  <si>
+    <t>Generar plan de proyecto y dar seguimiento con inconformidades de calidad asi como generar la asignación de tarea</t>
+  </si>
+  <si>
+    <t>Dar seguimiento a las ventas y seguir el proceso definido por la empresa</t>
+  </si>
+  <si>
+    <t>Realizar las actividades de soporte</t>
+  </si>
+  <si>
+    <t>Generar concentrados de metricas y estar en contacto con proveedores</t>
+  </si>
+  <si>
+    <t>Dirigir todas las areas de la empresa</t>
+  </si>
+  <si>
+    <t>no se requirio capacitación para la instalación del producto en ninguna de las areas requeridas</t>
+  </si>
+  <si>
+    <t>notificar actividad de implementación</t>
+  </si>
+  <si>
+    <t>Marisol Ornelas y Francisco Llamas</t>
+  </si>
+  <si>
+    <t>Dejar los sistemas configurados y funcionanco correctamente</t>
+  </si>
+  <si>
+    <t>1 vez por proyecto</t>
+  </si>
+  <si>
+    <t>notificar la finalización de la actividad agendada</t>
+  </si>
+  <si>
+    <t>Notificar que la tarea se finalizó con éxito</t>
+  </si>
+  <si>
+    <t>2 Computadoras</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>10 octubre del 2015</t>
+  </si>
+  <si>
+    <t>La fecha de obtención no aplica debido a que los equipos ya tienen bastante tiempo</t>
+  </si>
+  <si>
+    <t>2 licencias</t>
+  </si>
+  <si>
+    <t>17 octubre del 2015</t>
+  </si>
+  <si>
+    <t>17 de octubre del 2015</t>
+  </si>
+  <si>
+    <t>TeamViwer, Show myPC</t>
+  </si>
+  <si>
+    <t>Solicitar la instalación de TeamViwer o Show MyPC</t>
+  </si>
+  <si>
+    <t>Soporte</t>
+  </si>
+  <si>
+    <t>Falla de conexión remota con Ammyy Admin</t>
+  </si>
+  <si>
+    <t>Cerrado</t>
+  </si>
+  <si>
+    <t>1 ocación</t>
+  </si>
+  <si>
+    <t>Fallá en instalación y configuración del sistema</t>
+  </si>
+  <si>
+    <t>Validar los requerimientos minimos del equipo</t>
+  </si>
+  <si>
+    <t>Buscar y ejecutar la solución</t>
+  </si>
+  <si>
+    <t>Ocurrido</t>
+  </si>
+  <si>
+    <t>Fallas de descarga por baja potencia en internet del cliente</t>
+  </si>
+  <si>
+    <t>Validar que la descarga se halla realizado</t>
+  </si>
+  <si>
+    <t>Reagenda la cita</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>por evento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falla de servicio electrico </t>
+  </si>
+  <si>
+    <t>Comunicación con el cliente para reagendar cita</t>
+  </si>
+  <si>
+    <t>Home work</t>
+  </si>
+  <si>
+    <t>Falla de servicio de internet</t>
+  </si>
+  <si>
+    <t>Tener contrato con varias compañias de internet</t>
+  </si>
+  <si>
+    <t>Reportar el servicio fallido y cambiar la conexón de todas las maquinas</t>
+  </si>
+  <si>
+    <t>Mitigado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -708,6 +861,11 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1059,7 +1217,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1237,23 +1395,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1304,11 +1453,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1355,14 +1513,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1449,6 +1604,2765 @@
 </styleSheet>
 </file>
 
+<file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="accent1" pri="11200"/>
+  </dgm:catLst>
+  <dgm:styleLbl name="node0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="dk1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+</dgm:colorsDef>
+</file>
+
+<file path=xl/diagrams/data1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dgm:ptLst>
+    <dgm:pt modelId="{069B2C3C-A7DF-411E-99BB-50C754EEBBA8}" type="doc">
+      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1" loCatId="hierarchy" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="1"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{17F0494C-FD27-4FD1-A051-900A836B77E6}">
+      <dgm:prSet phldrT="[Texto]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX"/>
+            <a:t>Dirección</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FA86B3C4-935D-4EA6-B69D-3E508927E0A4}" type="parTrans" cxnId="{15ABE7F5-2842-4441-8A9B-B21DB4E7D6E2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{1A6A7697-9A91-407E-94B5-6C00854098E4}" type="sibTrans" cxnId="{15ABE7F5-2842-4441-8A9B-B21DB4E7D6E2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}">
+      <dgm:prSet phldrT="[Texto]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX"/>
+            <a:t>Administración</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" type="parTrans" cxnId="{587FC750-A57E-41E6-9C16-F15BDFC0AB68}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AF1B029C-996B-41F1-B71B-7831F8B05609}" type="sibTrans" cxnId="{587FC750-A57E-41E6-9C16-F15BDFC0AB68}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{BD914915-75E6-4220-A620-900406FDA3B2}">
+      <dgm:prSet phldrT="[Texto]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX"/>
+            <a:t>Ventas</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" type="parTrans" cxnId="{B10D13DE-BED0-4A3F-8A2A-CF05659F79FF}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{51991BF6-5A78-4A79-8F43-EDD763F7EB7F}" type="sibTrans" cxnId="{B10D13DE-BED0-4A3F-8A2A-CF05659F79FF}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}">
+      <dgm:prSet phldrT="[Texto]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX"/>
+            <a:t>Soporte</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2F3DE1A9-A637-43FB-B40F-F32225433690}" type="parTrans" cxnId="{BC7F4CE1-6BFB-4D0D-A759-BA2FB3CBAB7D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{11F25BED-BB76-46F3-9195-2189CEA15C24}" type="sibTrans" cxnId="{BC7F4CE1-6BFB-4D0D-A759-BA2FB3CBAB7D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}">
+      <dgm:prSet phldrT="[Texto]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX"/>
+            <a:t>Calidad</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" type="parTrans" cxnId="{44758180-DB92-4090-94C7-24FEFB1C4FF3}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DAE0CDDD-2988-4078-9851-07FA538106BA}" type="sibTrans" cxnId="{44758180-DB92-4090-94C7-24FEFB1C4FF3}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6EB61900-881E-4E1A-A687-35C7B965E9C9}" type="pres">
+      <dgm:prSet presAssocID="{069B2C3C-A7DF-411E-99BB-50C754EEBBA8}" presName="hierChild1" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="1"/>
+          <dgm:dir/>
+          <dgm:animOne val="branch"/>
+          <dgm:animLvl val="lvl"/>
+          <dgm:resizeHandles/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3766E119-5E72-46E5-9B3E-7281BD244EC0}" type="pres">
+      <dgm:prSet presAssocID="{17F0494C-FD27-4FD1-A051-900A836B77E6}" presName="hierRoot1" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F992707F-123D-4ADD-A0AF-9A81005FBDC8}" type="pres">
+      <dgm:prSet presAssocID="{17F0494C-FD27-4FD1-A051-900A836B77E6}" presName="composite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{57392886-85A9-4EF8-A46E-DAA437D58227}" type="pres">
+      <dgm:prSet presAssocID="{17F0494C-FD27-4FD1-A051-900A836B77E6}" presName="background" presStyleLbl="node0" presStyleIdx="0" presStyleCnt="1"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FAB54F49-6F1E-4DB1-AE8D-CA48304C119B}" type="pres">
+      <dgm:prSet presAssocID="{17F0494C-FD27-4FD1-A051-900A836B77E6}" presName="text" presStyleLbl="fgAcc0" presStyleIdx="0" presStyleCnt="1" custLinFactNeighborX="-901" custLinFactNeighborY="-15613">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{189A00CA-B097-43CA-9251-86C5E68833D2}" type="pres">
+      <dgm:prSet presAssocID="{17F0494C-FD27-4FD1-A051-900A836B77E6}" presName="hierChild2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{42E2241A-2870-46FF-8DCE-7CECD3E1329D}" type="pres">
+      <dgm:prSet presAssocID="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" presName="Name10" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{22724428-FAFA-47E3-8460-72AEED602114}" type="pres">
+      <dgm:prSet presAssocID="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" presName="hierRoot2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{4AC26E07-212D-4B0C-9765-DA46CC99AB14}" type="pres">
+      <dgm:prSet presAssocID="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" presName="composite2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1C82A8F0-B4C4-4529-95CA-C207369EB06A}" type="pres">
+      <dgm:prSet presAssocID="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" presName="background2" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{578B30D0-A478-4D3A-A8E7-ECCF36290258}" type="pres">
+      <dgm:prSet presAssocID="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" presName="text2" presStyleLbl="fgAcc2" presStyleIdx="0" presStyleCnt="2" custLinFactNeighborX="60386">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C2D26F2E-65BB-4D83-94D5-DC2997E6B0C9}" type="pres">
+      <dgm:prSet presAssocID="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" presName="hierChild3" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9388E48A-AF3C-4951-A9C7-354D7C5B2D66}" type="pres">
+      <dgm:prSet presAssocID="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" presName="Name17" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0874AE97-0B38-47BD-B891-644A90E6B3E4}" type="pres">
+      <dgm:prSet presAssocID="{BD914915-75E6-4220-A620-900406FDA3B2}" presName="hierRoot3" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1D054FD7-8731-4084-B285-E0279D8F2F8B}" type="pres">
+      <dgm:prSet presAssocID="{BD914915-75E6-4220-A620-900406FDA3B2}" presName="composite3" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2F756F22-3226-4432-8CCE-ACBF428E30DC}" type="pres">
+      <dgm:prSet presAssocID="{BD914915-75E6-4220-A620-900406FDA3B2}" presName="background3" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{19AAD1D5-355B-4333-A789-29AA5F4960C4}" type="pres">
+      <dgm:prSet presAssocID="{BD914915-75E6-4220-A620-900406FDA3B2}" presName="text3" presStyleLbl="fgAcc3" presStyleIdx="0" presStyleCnt="2">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{66D60DCC-E206-4C8E-A62D-0338CC62B0C4}" type="pres">
+      <dgm:prSet presAssocID="{BD914915-75E6-4220-A620-900406FDA3B2}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{A4D2AEED-6ABD-461C-B680-196AEA7BA247}" type="pres">
+      <dgm:prSet presAssocID="{2F3DE1A9-A637-43FB-B40F-F32225433690}" presName="Name17" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FDAA5A44-72A4-4724-B0B7-1EFECD3CE735}" type="pres">
+      <dgm:prSet presAssocID="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" presName="hierRoot3" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1F0EDBBE-B9AB-4BB2-AF3A-B73466017442}" type="pres">
+      <dgm:prSet presAssocID="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" presName="composite3" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F927FE6E-0C0B-4F07-A034-20A7B5D5E01C}" type="pres">
+      <dgm:prSet presAssocID="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" presName="background3" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{475D410A-9AE5-420A-8E06-1824378E493C}" type="pres">
+      <dgm:prSet presAssocID="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" presName="text3" presStyleLbl="fgAcc3" presStyleIdx="1" presStyleCnt="2">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C3D9C88F-3491-4A50-9C8B-CC58186AA0F0}" type="pres">
+      <dgm:prSet presAssocID="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E7DA8D89-CCA8-4F4E-AE9E-12E48D3F5441}" type="pres">
+      <dgm:prSet presAssocID="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" presName="Name10" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{20BE8ED7-D65A-4397-B5A3-79F2C7738123}" type="pres">
+      <dgm:prSet presAssocID="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" presName="hierRoot2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{ACB67E60-23BA-413E-98BA-FE158F6BDC50}" type="pres">
+      <dgm:prSet presAssocID="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" presName="composite2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{52B56B9A-A1DC-4F06-8715-BCE3AC67A3B7}" type="pres">
+      <dgm:prSet presAssocID="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" presName="background2" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8FFC4AEB-5DBD-41FD-BB16-9F9CA105399A}" type="pres">
+      <dgm:prSet presAssocID="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" presName="text2" presStyleLbl="fgAcc2" presStyleIdx="1" presStyleCnt="2" custLinFactY="47611" custLinFactNeighborX="52274" custLinFactNeighborY="100000">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3C01DC9C-BB9C-41AB-80FA-1E62D053CBEA}" type="pres">
+      <dgm:prSet presAssocID="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" presName="hierChild3" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+  </dgm:ptLst>
+  <dgm:cxnLst>
+    <dgm:cxn modelId="{90CC6FAC-59F3-45D3-8389-8903D5C28C61}" type="presOf" srcId="{BD914915-75E6-4220-A620-900406FDA3B2}" destId="{19AAD1D5-355B-4333-A789-29AA5F4960C4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{587FC750-A57E-41E6-9C16-F15BDFC0AB68}" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" srcOrd="0" destOrd="0" parTransId="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" sibTransId="{AF1B029C-996B-41F1-B71B-7831F8B05609}"/>
+    <dgm:cxn modelId="{61D5FC77-1C74-4BF6-B117-53E9D9FFA809}" type="presOf" srcId="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" destId="{42E2241A-2870-46FF-8DCE-7CECD3E1329D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{9156B689-2FE2-4B92-A4AE-B0769BCCD1A6}" type="presOf" srcId="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" destId="{8FFC4AEB-5DBD-41FD-BB16-9F9CA105399A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{BC7F4CE1-6BFB-4D0D-A759-BA2FB3CBAB7D}" srcId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" destId="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" srcOrd="1" destOrd="0" parTransId="{2F3DE1A9-A637-43FB-B40F-F32225433690}" sibTransId="{11F25BED-BB76-46F3-9195-2189CEA15C24}"/>
+    <dgm:cxn modelId="{6939BC63-54A1-4E46-A4D7-33B8E0B3FABB}" type="presOf" srcId="{2F3DE1A9-A637-43FB-B40F-F32225433690}" destId="{A4D2AEED-6ABD-461C-B680-196AEA7BA247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{15ABE7F5-2842-4441-8A9B-B21DB4E7D6E2}" srcId="{069B2C3C-A7DF-411E-99BB-50C754EEBBA8}" destId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" srcOrd="0" destOrd="0" parTransId="{FA86B3C4-935D-4EA6-B69D-3E508927E0A4}" sibTransId="{1A6A7697-9A91-407E-94B5-6C00854098E4}"/>
+    <dgm:cxn modelId="{5DBC543C-5BBF-454E-8905-B92A4ECF2025}" type="presOf" srcId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" destId="{578B30D0-A478-4D3A-A8E7-ECCF36290258}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{B10D13DE-BED0-4A3F-8A2A-CF05659F79FF}" srcId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" destId="{BD914915-75E6-4220-A620-900406FDA3B2}" srcOrd="0" destOrd="0" parTransId="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" sibTransId="{51991BF6-5A78-4A79-8F43-EDD763F7EB7F}"/>
+    <dgm:cxn modelId="{ACBAC60E-C45E-4B51-BFDD-C2E066DFC07C}" type="presOf" srcId="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" destId="{9388E48A-AF3C-4951-A9C7-354D7C5B2D66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{9BC0129D-F94A-4833-9964-064BED77EF68}" type="presOf" srcId="{069B2C3C-A7DF-411E-99BB-50C754EEBBA8}" destId="{6EB61900-881E-4E1A-A687-35C7B965E9C9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{44758180-DB92-4090-94C7-24FEFB1C4FF3}" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" srcOrd="1" destOrd="0" parTransId="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" sibTransId="{DAE0CDDD-2988-4078-9851-07FA538106BA}"/>
+    <dgm:cxn modelId="{3254A9F3-AB89-4B45-8AF7-D6BB4771BFDC}" type="presOf" srcId="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" destId="{E7DA8D89-CCA8-4F4E-AE9E-12E48D3F5441}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{841CFBA3-9F62-4BD5-A1AC-84D8AE636CDC}" type="presOf" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{FAB54F49-6F1E-4DB1-AE8D-CA48304C119B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{1006F441-2900-49CA-AE4C-A89FDA5A824D}" type="presOf" srcId="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" destId="{475D410A-9AE5-420A-8E06-1824378E493C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{3836A5FD-8F3A-4184-91AB-57736D0A77E7}" type="presParOf" srcId="{6EB61900-881E-4E1A-A687-35C7B965E9C9}" destId="{3766E119-5E72-46E5-9B3E-7281BD244EC0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{84A496A5-5252-471D-93EE-EC8FF72F091E}" type="presParOf" srcId="{3766E119-5E72-46E5-9B3E-7281BD244EC0}" destId="{F992707F-123D-4ADD-A0AF-9A81005FBDC8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{D82DEC92-9A1D-433B-890E-45869993FF24}" type="presParOf" srcId="{F992707F-123D-4ADD-A0AF-9A81005FBDC8}" destId="{57392886-85A9-4EF8-A46E-DAA437D58227}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{D0E78058-7DF8-46CD-B413-3D2B1C5AC96F}" type="presParOf" srcId="{F992707F-123D-4ADD-A0AF-9A81005FBDC8}" destId="{FAB54F49-6F1E-4DB1-AE8D-CA48304C119B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{16A8E209-2B96-4108-8559-B2E8F8C5C0B0}" type="presParOf" srcId="{3766E119-5E72-46E5-9B3E-7281BD244EC0}" destId="{189A00CA-B097-43CA-9251-86C5E68833D2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{BDAC0371-7BA3-4B25-AF20-947863F2A3E2}" type="presParOf" srcId="{189A00CA-B097-43CA-9251-86C5E68833D2}" destId="{42E2241A-2870-46FF-8DCE-7CECD3E1329D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{C720919D-DE1A-413D-9BFA-7046EDAD195E}" type="presParOf" srcId="{189A00CA-B097-43CA-9251-86C5E68833D2}" destId="{22724428-FAFA-47E3-8460-72AEED602114}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{C490A5B8-D697-44C1-92D6-18202FC7EA5D}" type="presParOf" srcId="{22724428-FAFA-47E3-8460-72AEED602114}" destId="{4AC26E07-212D-4B0C-9765-DA46CC99AB14}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{2711A94B-0232-4FFA-9A72-79DDF4497BC2}" type="presParOf" srcId="{4AC26E07-212D-4B0C-9765-DA46CC99AB14}" destId="{1C82A8F0-B4C4-4529-95CA-C207369EB06A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{4D26F704-0745-4272-ACFC-F3BCE1FBFDC8}" type="presParOf" srcId="{4AC26E07-212D-4B0C-9765-DA46CC99AB14}" destId="{578B30D0-A478-4D3A-A8E7-ECCF36290258}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{71B69FA0-0E3F-421D-AB8C-E9C4678BA523}" type="presParOf" srcId="{22724428-FAFA-47E3-8460-72AEED602114}" destId="{C2D26F2E-65BB-4D83-94D5-DC2997E6B0C9}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{36E91DAE-FF4A-4097-8D34-25D92162138F}" type="presParOf" srcId="{C2D26F2E-65BB-4D83-94D5-DC2997E6B0C9}" destId="{9388E48A-AF3C-4951-A9C7-354D7C5B2D66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{B7196FBE-D2FB-42A4-A0A8-8E921551D576}" type="presParOf" srcId="{C2D26F2E-65BB-4D83-94D5-DC2997E6B0C9}" destId="{0874AE97-0B38-47BD-B891-644A90E6B3E4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{6ECCA458-5BE1-4313-B457-21F18E2D7CF4}" type="presParOf" srcId="{0874AE97-0B38-47BD-B891-644A90E6B3E4}" destId="{1D054FD7-8731-4084-B285-E0279D8F2F8B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{EEB0EC67-2B26-467F-B986-5DD76EA37E3E}" type="presParOf" srcId="{1D054FD7-8731-4084-B285-E0279D8F2F8B}" destId="{2F756F22-3226-4432-8CCE-ACBF428E30DC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{99286E54-55CB-413F-9DE5-52947A1E2806}" type="presParOf" srcId="{1D054FD7-8731-4084-B285-E0279D8F2F8B}" destId="{19AAD1D5-355B-4333-A789-29AA5F4960C4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{66FF5479-4033-423E-A742-DC08E5838BD2}" type="presParOf" srcId="{0874AE97-0B38-47BD-B891-644A90E6B3E4}" destId="{66D60DCC-E206-4C8E-A62D-0338CC62B0C4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{B5C44A21-A09A-4EFB-958E-7E9F456027BE}" type="presParOf" srcId="{C2D26F2E-65BB-4D83-94D5-DC2997E6B0C9}" destId="{A4D2AEED-6ABD-461C-B680-196AEA7BA247}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{E89F3420-290B-4FA5-97B6-BA554E6DDC47}" type="presParOf" srcId="{C2D26F2E-65BB-4D83-94D5-DC2997E6B0C9}" destId="{FDAA5A44-72A4-4724-B0B7-1EFECD3CE735}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{BD4FDF45-B9E8-4DE1-B6A2-328738A5DA2E}" type="presParOf" srcId="{FDAA5A44-72A4-4724-B0B7-1EFECD3CE735}" destId="{1F0EDBBE-B9AB-4BB2-AF3A-B73466017442}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{8D247D63-4CDD-4E73-BEC2-617337586BD1}" type="presParOf" srcId="{1F0EDBBE-B9AB-4BB2-AF3A-B73466017442}" destId="{F927FE6E-0C0B-4F07-A034-20A7B5D5E01C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{A020E608-9DD2-4D6B-8FB4-0B7ABEDC513B}" type="presParOf" srcId="{1F0EDBBE-B9AB-4BB2-AF3A-B73466017442}" destId="{475D410A-9AE5-420A-8E06-1824378E493C}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{A140AC4B-88C7-4FB7-8352-DD1A14DDD12C}" type="presParOf" srcId="{FDAA5A44-72A4-4724-B0B7-1EFECD3CE735}" destId="{C3D9C88F-3491-4A50-9C8B-CC58186AA0F0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{9CDB6693-3B8C-440E-807B-972E09B87A88}" type="presParOf" srcId="{189A00CA-B097-43CA-9251-86C5E68833D2}" destId="{E7DA8D89-CCA8-4F4E-AE9E-12E48D3F5441}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{B49FA74A-F3BC-4A7F-814E-39291A63654B}" type="presParOf" srcId="{189A00CA-B097-43CA-9251-86C5E68833D2}" destId="{20BE8ED7-D65A-4397-B5A3-79F2C7738123}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{82B1D515-966F-4B59-B654-B3EFC0DB902C}" type="presParOf" srcId="{20BE8ED7-D65A-4397-B5A3-79F2C7738123}" destId="{ACB67E60-23BA-413E-98BA-FE158F6BDC50}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{CB1FFCDE-CB68-415C-A61B-B73432D479A7}" type="presParOf" srcId="{ACB67E60-23BA-413E-98BA-FE158F6BDC50}" destId="{52B56B9A-A1DC-4F06-8715-BCE3AC67A3B7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{AC36D4DF-74C8-44BC-A03C-69B3E0B82221}" type="presParOf" srcId="{ACB67E60-23BA-413E-98BA-FE158F6BDC50}" destId="{8FFC4AEB-5DBD-41FD-BB16-9F9CA105399A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{B791DBE6-9961-494B-990D-E0371C331640}" type="presParOf" srcId="{20BE8ED7-D65A-4397-B5A3-79F2C7738123}" destId="{3C01DC9C-BB9C-41AB-80FA-1E62D053CBEA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+  </dgm:cxnLst>
+  <dgm:bg/>
+  <dgm:whole/>
+</dgm:dataModel>
+</file>
+
+<file path=xl/diagrams/layout1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:layoutDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="hierarchy" pri="2000"/>
+  </dgm:catLst>
+  <dgm:sampData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="2">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="21">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="22">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="3">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="31">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="1" destId="2" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="1" destId="3" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="23" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="24" srcId="2" destId="22" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="33" srcId="3" destId="31" srcOrd="0" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:sampData>
+  <dgm:styleData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="11"/>
+        <dgm:pt modelId="12"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="2" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="13" srcId="1" destId="11" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="14" srcId="1" destId="12" srcOrd="1" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:styleData>
+  <dgm:clrData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="21"/>
+        <dgm:pt modelId="211"/>
+        <dgm:pt modelId="3"/>
+        <dgm:pt modelId="31"/>
+        <dgm:pt modelId="311"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="1" destId="2" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="1" destId="3" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="23" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="24" srcId="21" destId="211" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="33" srcId="3" destId="31" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="34" srcId="31" destId="311" srcOrd="0" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:clrData>
+  <dgm:layoutNode name="hierChild1">
+    <dgm:varLst>
+      <dgm:chPref val="1"/>
+      <dgm:dir/>
+      <dgm:animOne val="branch"/>
+      <dgm:animLvl val="lvl"/>
+      <dgm:resizeHandles/>
+    </dgm:varLst>
+    <dgm:choose name="Name0">
+      <dgm:if name="Name1" func="var" arg="dir" op="equ" val="norm">
+        <dgm:alg type="hierChild">
+          <dgm:param type="linDir" val="fromL"/>
+        </dgm:alg>
+      </dgm:if>
+      <dgm:else name="Name2">
+        <dgm:alg type="hierChild">
+          <dgm:param type="linDir" val="fromR"/>
+        </dgm:alg>
+      </dgm:else>
+    </dgm:choose>
+    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+      <dgm:adjLst/>
+    </dgm:shape>
+    <dgm:presOf/>
+    <dgm:constrLst>
+      <dgm:constr type="primFontSz" for="des" ptType="node" op="equ" val="65"/>
+      <dgm:constr type="w" for="des" forName="composite" refType="w"/>
+      <dgm:constr type="h" for="des" forName="composite" refType="w" refFor="des" refForName="composite" fact="0.667"/>
+      <dgm:constr type="w" for="des" forName="composite2" refType="w" refFor="des" refForName="composite"/>
+      <dgm:constr type="h" for="des" forName="composite2" refType="h" refFor="des" refForName="composite"/>
+      <dgm:constr type="w" for="des" forName="composite3" refType="w" refFor="des" refForName="composite"/>
+      <dgm:constr type="h" for="des" forName="composite3" refType="h" refFor="des" refForName="composite"/>
+      <dgm:constr type="w" for="des" forName="composite4" refType="w" refFor="des" refForName="composite"/>
+      <dgm:constr type="h" for="des" forName="composite4" refType="h" refFor="des" refForName="composite"/>
+      <dgm:constr type="w" for="des" forName="composite5" refType="w" refFor="des" refForName="composite"/>
+      <dgm:constr type="h" for="des" forName="composite5" refType="h" refFor="des" refForName="composite"/>
+      <dgm:constr type="sibSp" refType="w" refFor="des" refForName="composite" fact="0.1"/>
+      <dgm:constr type="sibSp" for="des" forName="hierChild2" refType="sibSp"/>
+      <dgm:constr type="sibSp" for="des" forName="hierChild3" refType="sibSp"/>
+      <dgm:constr type="sibSp" for="des" forName="hierChild4" refType="sibSp"/>
+      <dgm:constr type="sibSp" for="des" forName="hierChild5" refType="sibSp"/>
+      <dgm:constr type="sibSp" for="des" forName="hierChild6" refType="sibSp"/>
+      <dgm:constr type="sp" for="des" forName="hierRoot1" refType="h" refFor="des" refForName="composite" fact="0.25"/>
+      <dgm:constr type="sp" for="des" forName="hierRoot2" refType="sp" refFor="des" refForName="hierRoot1"/>
+      <dgm:constr type="sp" for="des" forName="hierRoot3" refType="sp" refFor="des" refForName="hierRoot1"/>
+      <dgm:constr type="sp" for="des" forName="hierRoot4" refType="sp" refFor="des" refForName="hierRoot1"/>
+      <dgm:constr type="sp" for="des" forName="hierRoot5" refType="sp" refFor="des" refForName="hierRoot1"/>
+    </dgm:constrLst>
+    <dgm:ruleLst/>
+    <dgm:forEach name="Name3" axis="ch">
+      <dgm:forEach name="Name4" axis="self" ptType="node">
+        <dgm:layoutNode name="hierRoot1">
+          <dgm:alg type="hierRoot"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf/>
+          <dgm:constrLst>
+            <dgm:constr type="bendDist" for="des" ptType="parTrans" refType="sp" fact="0.5"/>
+          </dgm:constrLst>
+          <dgm:ruleLst/>
+          <dgm:layoutNode name="composite">
+            <dgm:alg type="composite"/>
+            <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+              <dgm:adjLst/>
+            </dgm:shape>
+            <dgm:presOf/>
+            <dgm:constrLst>
+              <dgm:constr type="w" for="ch" forName="background" refType="w" fact="0.9"/>
+              <dgm:constr type="h" for="ch" forName="background" refType="w" refFor="ch" refForName="background" fact="0.635"/>
+              <dgm:constr type="t" for="ch" forName="background"/>
+              <dgm:constr type="l" for="ch" forName="background"/>
+              <dgm:constr type="w" for="ch" forName="text" refType="w" fact="0.9"/>
+              <dgm:constr type="h" for="ch" forName="text" refType="w" refFor="ch" refForName="text" fact="0.635"/>
+              <dgm:constr type="t" for="ch" forName="text" refType="w" fact="0.095"/>
+              <dgm:constr type="l" for="ch" forName="text" refType="w" fact="0.1"/>
+            </dgm:constrLst>
+            <dgm:ruleLst/>
+            <dgm:layoutNode name="background" styleLbl="node0" moveWith="text">
+              <dgm:alg type="sp"/>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                <dgm:adjLst>
+                  <dgm:adj idx="1" val="0.1"/>
+                </dgm:adjLst>
+              </dgm:shape>
+              <dgm:presOf/>
+              <dgm:constrLst/>
+              <dgm:ruleLst/>
+            </dgm:layoutNode>
+            <dgm:layoutNode name="text" styleLbl="fgAcc0">
+              <dgm:varLst>
+                <dgm:chPref val="3"/>
+              </dgm:varLst>
+              <dgm:alg type="tx"/>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                <dgm:adjLst>
+                  <dgm:adj idx="1" val="0.1"/>
+                </dgm:adjLst>
+              </dgm:shape>
+              <dgm:presOf axis="self"/>
+              <dgm:constrLst>
+                <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+              </dgm:constrLst>
+              <dgm:ruleLst>
+                <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+              </dgm:ruleLst>
+            </dgm:layoutNode>
+          </dgm:layoutNode>
+          <dgm:layoutNode name="hierChild2">
+            <dgm:choose name="Name5">
+              <dgm:if name="Name6" func="var" arg="dir" op="equ" val="norm">
+                <dgm:alg type="hierChild">
+                  <dgm:param type="linDir" val="fromL"/>
+                </dgm:alg>
+              </dgm:if>
+              <dgm:else name="Name7">
+                <dgm:alg type="hierChild">
+                  <dgm:param type="linDir" val="fromR"/>
+                </dgm:alg>
+              </dgm:else>
+            </dgm:choose>
+            <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+              <dgm:adjLst/>
+            </dgm:shape>
+            <dgm:presOf/>
+            <dgm:constrLst/>
+            <dgm:ruleLst/>
+            <dgm:forEach name="Name8" axis="ch">
+              <dgm:forEach name="Name9" axis="self" ptType="parTrans" cnt="1">
+                <dgm:layoutNode name="Name10">
+                  <dgm:alg type="conn">
+                    <dgm:param type="dim" val="1D"/>
+                    <dgm:param type="endSty" val="noArr"/>
+                    <dgm:param type="connRout" val="bend"/>
+                    <dgm:param type="bendPt" val="end"/>
+                    <dgm:param type="begPts" val="bCtr"/>
+                    <dgm:param type="endPts" val="tCtr"/>
+                    <dgm:param type="srcNode" val="background"/>
+                    <dgm:param type="dstNode" val="background2"/>
+                  </dgm:alg>
+                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="conn" r:blip="" zOrderOff="-999">
+                    <dgm:adjLst/>
+                  </dgm:shape>
+                  <dgm:presOf axis="self"/>
+                  <dgm:constrLst>
+                    <dgm:constr type="begPad"/>
+                    <dgm:constr type="endPad"/>
+                  </dgm:constrLst>
+                  <dgm:ruleLst/>
+                </dgm:layoutNode>
+              </dgm:forEach>
+              <dgm:forEach name="Name11" axis="self" ptType="node">
+                <dgm:layoutNode name="hierRoot2">
+                  <dgm:alg type="hierRoot"/>
+                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                    <dgm:adjLst/>
+                  </dgm:shape>
+                  <dgm:presOf/>
+                  <dgm:constrLst>
+                    <dgm:constr type="bendDist" for="des" ptType="parTrans" refType="sp" fact="0.5"/>
+                  </dgm:constrLst>
+                  <dgm:ruleLst/>
+                  <dgm:layoutNode name="composite2">
+                    <dgm:alg type="composite"/>
+                    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                      <dgm:adjLst/>
+                    </dgm:shape>
+                    <dgm:presOf/>
+                    <dgm:constrLst>
+                      <dgm:constr type="w" for="ch" forName="background2" refType="w" fact="0.9"/>
+                      <dgm:constr type="h" for="ch" forName="background2" refType="w" refFor="ch" refForName="background2" fact="0.635"/>
+                      <dgm:constr type="t" for="ch" forName="background2"/>
+                      <dgm:constr type="l" for="ch" forName="background2"/>
+                      <dgm:constr type="w" for="ch" forName="text2" refType="w" fact="0.9"/>
+                      <dgm:constr type="h" for="ch" forName="text2" refType="w" refFor="ch" refForName="text2" fact="0.635"/>
+                      <dgm:constr type="t" for="ch" forName="text2" refType="w" fact="0.095"/>
+                      <dgm:constr type="l" for="ch" forName="text2" refType="w" fact="0.1"/>
+                    </dgm:constrLst>
+                    <dgm:ruleLst/>
+                    <dgm:layoutNode name="background2" moveWith="text2">
+                      <dgm:alg type="sp"/>
+                      <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                        <dgm:adjLst>
+                          <dgm:adj idx="1" val="0.1"/>
+                        </dgm:adjLst>
+                      </dgm:shape>
+                      <dgm:presOf/>
+                      <dgm:constrLst/>
+                      <dgm:ruleLst/>
+                    </dgm:layoutNode>
+                    <dgm:layoutNode name="text2" styleLbl="fgAcc2">
+                      <dgm:varLst>
+                        <dgm:chPref val="3"/>
+                      </dgm:varLst>
+                      <dgm:alg type="tx"/>
+                      <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                        <dgm:adjLst>
+                          <dgm:adj idx="1" val="0.1"/>
+                        </dgm:adjLst>
+                      </dgm:shape>
+                      <dgm:presOf axis="self"/>
+                      <dgm:constrLst>
+                        <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+                        <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+                        <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+                        <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+                      </dgm:constrLst>
+                      <dgm:ruleLst>
+                        <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+                      </dgm:ruleLst>
+                    </dgm:layoutNode>
+                  </dgm:layoutNode>
+                  <dgm:layoutNode name="hierChild3">
+                    <dgm:choose name="Name12">
+                      <dgm:if name="Name13" func="var" arg="dir" op="equ" val="norm">
+                        <dgm:alg type="hierChild">
+                          <dgm:param type="linDir" val="fromL"/>
+                        </dgm:alg>
+                      </dgm:if>
+                      <dgm:else name="Name14">
+                        <dgm:alg type="hierChild">
+                          <dgm:param type="linDir" val="fromR"/>
+                        </dgm:alg>
+                      </dgm:else>
+                    </dgm:choose>
+                    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                      <dgm:adjLst/>
+                    </dgm:shape>
+                    <dgm:presOf/>
+                    <dgm:constrLst/>
+                    <dgm:ruleLst/>
+                    <dgm:forEach name="Name15" axis="ch">
+                      <dgm:forEach name="Name16" axis="self" ptType="parTrans" cnt="1">
+                        <dgm:layoutNode name="Name17">
+                          <dgm:alg type="conn">
+                            <dgm:param type="dim" val="1D"/>
+                            <dgm:param type="endSty" val="noArr"/>
+                            <dgm:param type="connRout" val="bend"/>
+                            <dgm:param type="bendPt" val="end"/>
+                            <dgm:param type="begPts" val="bCtr"/>
+                            <dgm:param type="endPts" val="tCtr"/>
+                            <dgm:param type="srcNode" val="background2"/>
+                            <dgm:param type="dstNode" val="background3"/>
+                          </dgm:alg>
+                          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="conn" r:blip="" zOrderOff="-999">
+                            <dgm:adjLst/>
+                          </dgm:shape>
+                          <dgm:presOf axis="self"/>
+                          <dgm:constrLst>
+                            <dgm:constr type="begPad"/>
+                            <dgm:constr type="endPad"/>
+                          </dgm:constrLst>
+                          <dgm:ruleLst/>
+                        </dgm:layoutNode>
+                      </dgm:forEach>
+                      <dgm:forEach name="Name18" axis="self" ptType="node">
+                        <dgm:layoutNode name="hierRoot3">
+                          <dgm:alg type="hierRoot"/>
+                          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                            <dgm:adjLst/>
+                          </dgm:shape>
+                          <dgm:presOf/>
+                          <dgm:constrLst>
+                            <dgm:constr type="bendDist" for="des" ptType="parTrans" refType="sp" fact="0.5"/>
+                          </dgm:constrLst>
+                          <dgm:ruleLst/>
+                          <dgm:layoutNode name="composite3">
+                            <dgm:alg type="composite"/>
+                            <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                              <dgm:adjLst/>
+                            </dgm:shape>
+                            <dgm:presOf/>
+                            <dgm:constrLst>
+                              <dgm:constr type="w" for="ch" forName="background3" refType="w" fact="0.9"/>
+                              <dgm:constr type="h" for="ch" forName="background3" refType="w" refFor="ch" refForName="background3" fact="0.635"/>
+                              <dgm:constr type="t" for="ch" forName="background3"/>
+                              <dgm:constr type="l" for="ch" forName="background3"/>
+                              <dgm:constr type="w" for="ch" forName="text3" refType="w" fact="0.9"/>
+                              <dgm:constr type="h" for="ch" forName="text3" refType="w" refFor="ch" refForName="text3" fact="0.635"/>
+                              <dgm:constr type="t" for="ch" forName="text3" refType="w" fact="0.095"/>
+                              <dgm:constr type="l" for="ch" forName="text3" refType="w" fact="0.1"/>
+                            </dgm:constrLst>
+                            <dgm:ruleLst/>
+                            <dgm:layoutNode name="background3" moveWith="text3">
+                              <dgm:alg type="sp"/>
+                              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                                <dgm:adjLst>
+                                  <dgm:adj idx="1" val="0.1"/>
+                                </dgm:adjLst>
+                              </dgm:shape>
+                              <dgm:presOf/>
+                              <dgm:constrLst/>
+                              <dgm:ruleLst/>
+                            </dgm:layoutNode>
+                            <dgm:layoutNode name="text3" styleLbl="fgAcc3">
+                              <dgm:varLst>
+                                <dgm:chPref val="3"/>
+                              </dgm:varLst>
+                              <dgm:alg type="tx"/>
+                              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                                <dgm:adjLst>
+                                  <dgm:adj idx="1" val="0.1"/>
+                                </dgm:adjLst>
+                              </dgm:shape>
+                              <dgm:presOf axis="self"/>
+                              <dgm:constrLst>
+                                <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+                                <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+                                <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+                                <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+                              </dgm:constrLst>
+                              <dgm:ruleLst>
+                                <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+                              </dgm:ruleLst>
+                            </dgm:layoutNode>
+                          </dgm:layoutNode>
+                          <dgm:layoutNode name="hierChild4">
+                            <dgm:choose name="Name19">
+                              <dgm:if name="Name20" func="var" arg="dir" op="equ" val="norm">
+                                <dgm:alg type="hierChild">
+                                  <dgm:param type="linDir" val="fromL"/>
+                                </dgm:alg>
+                              </dgm:if>
+                              <dgm:else name="Name21">
+                                <dgm:alg type="hierChild">
+                                  <dgm:param type="linDir" val="fromR"/>
+                                </dgm:alg>
+                              </dgm:else>
+                            </dgm:choose>
+                            <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                              <dgm:adjLst/>
+                            </dgm:shape>
+                            <dgm:presOf/>
+                            <dgm:constrLst/>
+                            <dgm:ruleLst/>
+                            <dgm:forEach name="repeat" axis="ch">
+                              <dgm:forEach name="Name22" axis="self" ptType="parTrans" cnt="1">
+                                <dgm:layoutNode name="Name23">
+                                  <dgm:choose name="Name24">
+                                    <dgm:if name="Name25" axis="self" func="depth" op="lte" val="4">
+                                      <dgm:alg type="conn">
+                                        <dgm:param type="dim" val="1D"/>
+                                        <dgm:param type="endSty" val="noArr"/>
+                                        <dgm:param type="connRout" val="bend"/>
+                                        <dgm:param type="bendPt" val="end"/>
+                                        <dgm:param type="begPts" val="bCtr"/>
+                                        <dgm:param type="endPts" val="tCtr"/>
+                                        <dgm:param type="srcNode" val="background3"/>
+                                        <dgm:param type="dstNode" val="background4"/>
+                                      </dgm:alg>
+                                    </dgm:if>
+                                    <dgm:else name="Name26">
+                                      <dgm:alg type="conn">
+                                        <dgm:param type="dim" val="1D"/>
+                                        <dgm:param type="endSty" val="noArr"/>
+                                        <dgm:param type="connRout" val="bend"/>
+                                        <dgm:param type="bendPt" val="end"/>
+                                        <dgm:param type="begPts" val="bCtr"/>
+                                        <dgm:param type="endPts" val="tCtr"/>
+                                        <dgm:param type="srcNode" val="background4"/>
+                                        <dgm:param type="dstNode" val="background4"/>
+                                      </dgm:alg>
+                                    </dgm:else>
+                                  </dgm:choose>
+                                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="conn" r:blip="" zOrderOff="-999">
+                                    <dgm:adjLst/>
+                                  </dgm:shape>
+                                  <dgm:presOf axis="self"/>
+                                  <dgm:constrLst>
+                                    <dgm:constr type="begPad"/>
+                                    <dgm:constr type="endPad"/>
+                                  </dgm:constrLst>
+                                  <dgm:ruleLst/>
+                                </dgm:layoutNode>
+                              </dgm:forEach>
+                              <dgm:forEach name="Name27" axis="self" ptType="node">
+                                <dgm:layoutNode name="hierRoot4">
+                                  <dgm:alg type="hierRoot"/>
+                                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                                    <dgm:adjLst/>
+                                  </dgm:shape>
+                                  <dgm:presOf/>
+                                  <dgm:constrLst>
+                                    <dgm:constr type="bendDist" for="des" ptType="parTrans" refType="sp" fact="0.5"/>
+                                  </dgm:constrLst>
+                                  <dgm:ruleLst/>
+                                  <dgm:layoutNode name="composite4">
+                                    <dgm:alg type="composite"/>
+                                    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                                      <dgm:adjLst/>
+                                    </dgm:shape>
+                                    <dgm:presOf/>
+                                    <dgm:constrLst>
+                                      <dgm:constr type="w" for="ch" forName="background4" refType="w" fact="0.9"/>
+                                      <dgm:constr type="h" for="ch" forName="background4" refType="w" refFor="ch" refForName="background4" fact="0.635"/>
+                                      <dgm:constr type="t" for="ch" forName="background4"/>
+                                      <dgm:constr type="l" for="ch" forName="background4"/>
+                                      <dgm:constr type="w" for="ch" forName="text4" refType="w" fact="0.9"/>
+                                      <dgm:constr type="h" for="ch" forName="text4" refType="w" refFor="ch" refForName="text4" fact="0.635"/>
+                                      <dgm:constr type="t" for="ch" forName="text4" refType="w" fact="0.095"/>
+                                      <dgm:constr type="l" for="ch" forName="text4" refType="w" fact="0.1"/>
+                                    </dgm:constrLst>
+                                    <dgm:ruleLst/>
+                                    <dgm:layoutNode name="background4" moveWith="text4">
+                                      <dgm:alg type="sp"/>
+                                      <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                                        <dgm:adjLst>
+                                          <dgm:adj idx="1" val="0.1"/>
+                                        </dgm:adjLst>
+                                      </dgm:shape>
+                                      <dgm:presOf/>
+                                      <dgm:constrLst/>
+                                      <dgm:ruleLst/>
+                                    </dgm:layoutNode>
+                                    <dgm:layoutNode name="text4" styleLbl="fgAcc4">
+                                      <dgm:varLst>
+                                        <dgm:chPref val="3"/>
+                                      </dgm:varLst>
+                                      <dgm:alg type="tx"/>
+                                      <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                                        <dgm:adjLst>
+                                          <dgm:adj idx="1" val="0.1"/>
+                                        </dgm:adjLst>
+                                      </dgm:shape>
+                                      <dgm:presOf axis="self"/>
+                                      <dgm:constrLst>
+                                        <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+                                        <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+                                        <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+                                        <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+                                      </dgm:constrLst>
+                                      <dgm:ruleLst>
+                                        <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+                                      </dgm:ruleLst>
+                                    </dgm:layoutNode>
+                                  </dgm:layoutNode>
+                                  <dgm:layoutNode name="hierChild5">
+                                    <dgm:choose name="Name28">
+                                      <dgm:if name="Name29" func="var" arg="dir" op="equ" val="norm">
+                                        <dgm:alg type="hierChild">
+                                          <dgm:param type="linDir" val="fromL"/>
+                                        </dgm:alg>
+                                      </dgm:if>
+                                      <dgm:else name="Name30">
+                                        <dgm:alg type="hierChild">
+                                          <dgm:param type="linDir" val="fromR"/>
+                                        </dgm:alg>
+                                      </dgm:else>
+                                    </dgm:choose>
+                                    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                                      <dgm:adjLst/>
+                                    </dgm:shape>
+                                    <dgm:presOf/>
+                                    <dgm:constrLst/>
+                                    <dgm:ruleLst/>
+                                    <dgm:forEach name="Name31" ref="repeat"/>
+                                  </dgm:layoutNode>
+                                </dgm:layoutNode>
+                              </dgm:forEach>
+                            </dgm:forEach>
+                          </dgm:layoutNode>
+                        </dgm:layoutNode>
+                      </dgm:forEach>
+                    </dgm:forEach>
+                  </dgm:layoutNode>
+                </dgm:layoutNode>
+              </dgm:forEach>
+            </dgm:forEach>
+          </dgm:layoutNode>
+        </dgm:layoutNode>
+      </dgm:forEach>
+    </dgm:forEach>
+  </dgm:layoutNode>
+</dgm:layoutDef>
+</file>
+
+<file path=xl/diagrams/quickStyle1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="simple" pri="10100"/>
+  </dgm:catLst>
+  <dgm:scene3d>
+    <a:camera prst="orthographicFront"/>
+    <a:lightRig rig="threePt" dir="t"/>
+  </dgm:scene3d>
+  <dgm:styleLbl name="node0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="tx1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+</dgm:styleDef>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1504,13 +4418,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1089000</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>91335</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>959040</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>91695</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1550,13 +4464,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>822600</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>129975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2315160</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>130335</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1590,6 +4504,36 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1857375</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="4 Diagrama"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+          <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId1" r:lo="rId2" r:qs="rId3" r:cs="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2370,8 +5314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMH8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2412,19 +5356,19 @@
       <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="111" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="112"/>
+      <c r="C2" s="111"/>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1">
       <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="111" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="112"/>
+      <c r="C3" s="111"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" customHeight="1">
       <c r="A4" s="114" t="s">
@@ -2437,34 +5381,34 @@
       <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="112"/>
+      <c r="C5" s="111"/>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1">
       <c r="A6" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="111">
+      <c r="B6" s="110">
         <v>42284</v>
       </c>
-      <c r="C6" s="111"/>
+      <c r="C6" s="110"/>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1">
       <c r="A7" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="112"/>
+      <c r="C7" s="111"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="128">
+      <c r="B8" s="112">
         <v>42321</v>
       </c>
       <c r="C8" s="113"/>
@@ -2489,7 +5433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A23" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -4596,10 +7540,10 @@
       <c r="D5"/>
     </row>
     <row r="6" spans="1:1024" ht="42.75" customHeight="1">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="111" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="112"/>
+      <c r="B6" s="111"/>
       <c r="C6"/>
       <c r="D6"/>
     </row>
@@ -4612,10 +7556,10 @@
       <c r="D7"/>
     </row>
     <row r="8" spans="1:1024" ht="146.25" customHeight="1">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="111" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="112"/>
+      <c r="B8" s="111"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
@@ -4631,7 +7575,7 @@
       <c r="A10" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="105" t="s">
         <v>83</v>
       </c>
       <c r="C10"/>
@@ -4641,7 +7585,7 @@
       <c r="A11" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="105" t="s">
         <v>101</v>
       </c>
       <c r="C11"/>
@@ -4651,7 +7595,7 @@
       <c r="A12" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="105" t="s">
         <v>102</v>
       </c>
       <c r="C12"/>
@@ -4692,10 +7636,10 @@
       <c r="B16" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="130">
+      <c r="C16" s="109">
         <v>42287</v>
       </c>
-      <c r="D16" s="130">
+      <c r="D16" s="109">
         <v>42321</v>
       </c>
     </row>
@@ -4703,13 +7647,13 @@
       <c r="A17" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="130">
+      <c r="C17" s="109">
         <v>42325</v>
       </c>
-      <c r="D17" s="130"/>
+      <c r="D17" s="109"/>
     </row>
     <row r="18" spans="1:4" outlineLevel="1">
       <c r="A18" s="3" t="s">
@@ -4718,7 +7662,7 @@
       <c r="B18" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="130">
+      <c r="C18" s="109">
         <v>42325</v>
       </c>
       <c r="D18" s="83"/>
@@ -4799,21 +7743,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4825,7 +7769,7 @@
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -5889,13 +8833,13 @@
       <c r="AMI1"/>
     </row>
     <row r="2" spans="1:1024" ht="18.75">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -6916,53 +9860,73 @@
       <c r="AMI2"/>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="18" customHeight="1" outlineLevel="1">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="106" t="s">
+      <c r="E3" s="103" t="s">
         <v>29</v>
       </c>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" outlineLevel="1">
-      <c r="A4" s="97" t="s">
+    <row r="4" spans="1:1024" ht="25.5" outlineLevel="1">
+      <c r="A4" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="107"/>
+      <c r="C4" s="94" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="104" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5" spans="1:1024" outlineLevel="1">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="107"/>
+      <c r="C5" s="94">
+        <v>3313482553</v>
+      </c>
+      <c r="D5" s="106" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="104" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="6" spans="1:1024" outlineLevel="1">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="78"/>
+      <c r="B6" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="78" t="s">
+        <v>121</v>
+      </c>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
@@ -7983,62 +10947,76 @@
       <c r="AMI6"/>
     </row>
     <row r="7" spans="1:1024" ht="25.5" outlineLevel="1">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="94" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="97"/>
-      <c r="D7" s="109" t="s">
+      <c r="C7" s="94">
+        <v>3318039095</v>
+      </c>
+      <c r="D7" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="110" t="s">
+      <c r="E7" s="107" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:1024" outlineLevel="1">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="97" t="s">
+      <c r="B8" s="94" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="78"/>
+      <c r="C8" s="94" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="106" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="78" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="9" spans="1:1024" outlineLevel="1">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="94" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="97"/>
-      <c r="E9" s="78"/>
+      <c r="C9" s="94">
+        <v>3312448000</v>
+      </c>
+      <c r="D9" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="78" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="10" spans="1:1024" outlineLevel="1">
-      <c r="A10" s="97"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
+      <c r="A10" s="94"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:1024" outlineLevel="1">
-      <c r="A11" s="97"/>
-      <c r="B11" s="97"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="97"/>
+      <c r="A11" s="94"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
     </row>
     <row r="12" spans="1:1024" outlineLevel="1">
-      <c r="A12" s="97"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
+      <c r="A12" s="94"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
@@ -9059,24 +12037,24 @@
       <c r="AMI12"/>
     </row>
     <row r="13" spans="1:1024" outlineLevel="1">
-      <c r="A13" s="97"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
     </row>
     <row r="14" spans="1:1024" outlineLevel="1">
-      <c r="A14" s="97"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
     </row>
     <row r="15" spans="1:1024" outlineLevel="1">
-      <c r="A15" s="101"/>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
       <c r="E15" s="81"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -10118,10 +13096,15 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -10129,8 +13112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -10160,19 +13143,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="38.25">
       <c r="A2" s="87"/>
       <c r="B2" s="87"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
+      <c r="C2" s="128" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="87"/>
       <c r="B3" s="87"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="87"/>
@@ -10253,7 +13238,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -12361,19 +15346,19 @@
       <c r="AMI2"/>
     </row>
     <row r="3" spans="1:1024">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="89" t="s">
         <v>40</v>
       </c>
       <c r="F3"/>
@@ -13395,12 +16380,22 @@
       <c r="AMH3"/>
       <c r="AMI3"/>
     </row>
-    <row r="4" spans="1:1024">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
+    <row r="4" spans="1:1024" ht="25.5">
+      <c r="A4" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="92" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="90" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="92" t="s">
+        <v>128</v>
+      </c>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -14420,66 +17415,76 @@
       <c r="AMH4"/>
       <c r="AMI4"/>
     </row>
-    <row r="5" spans="1:1024" s="8" customFormat="1">
-      <c r="A5" s="94"/>
-      <c r="B5" s="95"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="95"/>
+    <row r="5" spans="1:1024" s="8" customFormat="1" ht="25.5">
+      <c r="A5" s="91" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="90" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="92" t="s">
+        <v>128</v>
+      </c>
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1024" s="8" customFormat="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="95"/>
+      <c r="A6" s="129"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024" s="8" customFormat="1">
-      <c r="A7" s="94"/>
-      <c r="B7" s="95"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="95"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="92"/>
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1024" s="8" customFormat="1">
-      <c r="A8" s="94"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="95"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="92"/>
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" s="8" customFormat="1">
-      <c r="A9" s="94"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="95"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="92"/>
       <c r="AMJ9"/>
     </row>
     <row r="10" spans="1:1024">
-      <c r="A10" s="94"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
     </row>
     <row r="11" spans="1:1024">
-      <c r="A11" s="94"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IT5:IT11 SP5:SP11 ACL5:ACL11 AMH5:AMH11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IT5:IT11 AMH5:AMH11 ACL5:ACL11 SP5:SP11">
       <formula1>"Orientación,Reporte,Reunión Periódica"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -14496,7 +17501,7 @@
   <dimension ref="A1:AMI15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -14560,123 +17565,151 @@
       </c>
       <c r="J3"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="96"/>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="97"/>
+    <row r="4" spans="1:10" ht="51">
+      <c r="A4" s="93" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="94" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="94">
+        <v>2</v>
+      </c>
+      <c r="E4" s="95" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="95" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="94" t="s">
+        <v>134</v>
+      </c>
       <c r="J4" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="96"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="97"/>
+    <row r="5" spans="1:10" ht="38.25">
+      <c r="A5" s="93" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="94">
+        <v>2</v>
+      </c>
+      <c r="E5" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="95" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="94" t="s">
+        <v>132</v>
+      </c>
       <c r="J5" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="96"/>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="97"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="94"/>
       <c r="J6" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="96"/>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="97"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="94"/>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="96"/>
-      <c r="B8" s="97"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="97"/>
+      <c r="A8" s="93"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="95"/>
+      <c r="G8" s="94"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="99"/>
-      <c r="B9" s="97"/>
-      <c r="C9" s="97"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="97"/>
+      <c r="A9" s="96"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="94"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="96"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="97"/>
+      <c r="A10" s="93"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="94"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="96"/>
-      <c r="B11" s="97"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="97"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="94"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="96"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="97"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="94"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="97"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="97"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="97"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14700,7 +17733,7 @@
   <dimension ref="A1:AMK43"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -15874,25 +18907,41 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" ht="15">
+    <row r="5" spans="1:1024" ht="25.5">
       <c r="A5" s="24">
         <v>1</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="24">
+        <v>1</v>
+      </c>
       <c r="D5" s="26">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E5" s="24">
         <f>PRODUCT(A5:D5)</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="F5" s="24">
+        <v>4</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>152</v>
+      </c>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
@@ -16907,23 +19956,41 @@
       <c r="AMI5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1024" ht="15">
+    <row r="6" spans="1:1024" ht="25.5">
       <c r="A6" s="24">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="24">
+        <v>4</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0.2</v>
+      </c>
       <c r="E6" s="24">
         <f t="shared" ref="E6:E24" si="0">PRODUCT(C6:D6)</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
+      <c r="F6" s="24">
+        <v>3</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>143</v>
+      </c>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6"/>
@@ -17938,23 +21005,41 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" ht="15">
+    <row r="7" spans="1:1024" ht="25.5">
       <c r="A7" s="24">
         <v>3</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="24">
+        <v>4</v>
+      </c>
+      <c r="D7" s="26">
+        <v>0.2</v>
+      </c>
       <c r="E7" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="29"/>
+      <c r="F7" s="24">
+        <v>3</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>152</v>
+      </c>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -18973,19 +22058,37 @@
       <c r="A8" s="24">
         <v>4</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="24">
+        <v>5</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0.01</v>
+      </c>
       <c r="E8" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="29"/>
+      <c r="F8" s="24">
+        <v>4</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>132</v>
+      </c>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
@@ -20004,19 +23107,37 @@
       <c r="A9" s="24">
         <v>5</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="26"/>
+      <c r="B9" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="24">
+        <v>5</v>
+      </c>
+      <c r="D9" s="26">
+        <v>0.05</v>
+      </c>
       <c r="E9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="29"/>
+      <c r="F9" s="24">
+        <v>4</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>132</v>
+      </c>
       <c r="L9"/>
       <c r="M9"/>
       <c r="N9"/>

</xml_diff>

<commit_message>
correccion de no conformidades
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1319 - CCON,CNOM, Jeniffer Venegas _MO/Planeación/Plan_de_proyecto.xlsx
+++ b/Proyectos/2015/11/P1319 - CCON,CNOM, Jeniffer Venegas _MO/Planeación/Plan_de_proyecto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-60" windowWidth="16380" windowHeight="8250" tabRatio="875"/>
+    <workbookView xWindow="0" yWindow="-60" windowWidth="16380" windowHeight="8250" tabRatio="875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" r:id="rId1"/>
@@ -1459,6 +1459,12 @@
     <xf numFmtId="14" fontId="20" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1512,12 +1518,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2556,6 +2556,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{3766E119-5E72-46E5-9B3E-7281BD244EC0}" type="pres">
       <dgm:prSet presAssocID="{17F0494C-FD27-4FD1-A051-900A836B77E6}" presName="hierRoot1" presStyleCnt="0"/>
@@ -2591,6 +2598,13 @@
     <dgm:pt modelId="{42E2241A-2870-46FF-8DCE-7CECD3E1329D}" type="pres">
       <dgm:prSet presAssocID="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" presName="Name10" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{22724428-FAFA-47E3-8460-72AEED602114}" type="pres">
       <dgm:prSet presAssocID="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" presName="hierRoot2" presStyleCnt="0"/>
@@ -2626,6 +2640,13 @@
     <dgm:pt modelId="{9388E48A-AF3C-4951-A9C7-354D7C5B2D66}" type="pres">
       <dgm:prSet presAssocID="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" presName="Name17" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0874AE97-0B38-47BD-B891-644A90E6B3E4}" type="pres">
       <dgm:prSet presAssocID="{BD914915-75E6-4220-A620-900406FDA3B2}" presName="hierRoot3" presStyleCnt="0"/>
@@ -2661,6 +2682,13 @@
     <dgm:pt modelId="{A4D2AEED-6ABD-461C-B680-196AEA7BA247}" type="pres">
       <dgm:prSet presAssocID="{2F3DE1A9-A637-43FB-B40F-F32225433690}" presName="Name17" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{FDAA5A44-72A4-4724-B0B7-1EFECD3CE735}" type="pres">
       <dgm:prSet presAssocID="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" presName="hierRoot3" presStyleCnt="0"/>
@@ -2681,6 +2709,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C3D9C88F-3491-4A50-9C8B-CC58186AA0F0}" type="pres">
       <dgm:prSet presAssocID="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" presName="hierChild4" presStyleCnt="0"/>
@@ -2689,6 +2724,13 @@
     <dgm:pt modelId="{E7DA8D89-CCA8-4F4E-AE9E-12E48D3F5441}" type="pres">
       <dgm:prSet presAssocID="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" presName="Name10" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{20BE8ED7-D65A-4397-B5A3-79F2C7738123}" type="pres">
       <dgm:prSet presAssocID="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" presName="hierRoot2" presStyleCnt="0"/>
@@ -2709,6 +2751,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{3C01DC9C-BB9C-41AB-80FA-1E62D053CBEA}" type="pres">
       <dgm:prSet presAssocID="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" presName="hierChild3" presStyleCnt="0"/>
@@ -2716,20 +2765,20 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{9BC0129D-F94A-4833-9964-064BED77EF68}" type="presOf" srcId="{069B2C3C-A7DF-411E-99BB-50C754EEBBA8}" destId="{6EB61900-881E-4E1A-A687-35C7B965E9C9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{841CFBA3-9F62-4BD5-A1AC-84D8AE636CDC}" type="presOf" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{FAB54F49-6F1E-4DB1-AE8D-CA48304C119B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{90CC6FAC-59F3-45D3-8389-8903D5C28C61}" type="presOf" srcId="{BD914915-75E6-4220-A620-900406FDA3B2}" destId="{19AAD1D5-355B-4333-A789-29AA5F4960C4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
-    <dgm:cxn modelId="{587FC750-A57E-41E6-9C16-F15BDFC0AB68}" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" srcOrd="0" destOrd="0" parTransId="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" sibTransId="{AF1B029C-996B-41F1-B71B-7831F8B05609}"/>
-    <dgm:cxn modelId="{61D5FC77-1C74-4BF6-B117-53E9D9FFA809}" type="presOf" srcId="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" destId="{42E2241A-2870-46FF-8DCE-7CECD3E1329D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{9156B689-2FE2-4B92-A4AE-B0769BCCD1A6}" type="presOf" srcId="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" destId="{8FFC4AEB-5DBD-41FD-BB16-9F9CA105399A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{BC7F4CE1-6BFB-4D0D-A759-BA2FB3CBAB7D}" srcId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" destId="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" srcOrd="1" destOrd="0" parTransId="{2F3DE1A9-A637-43FB-B40F-F32225433690}" sibTransId="{11F25BED-BB76-46F3-9195-2189CEA15C24}"/>
     <dgm:cxn modelId="{6939BC63-54A1-4E46-A4D7-33B8E0B3FABB}" type="presOf" srcId="{2F3DE1A9-A637-43FB-B40F-F32225433690}" destId="{A4D2AEED-6ABD-461C-B680-196AEA7BA247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{ACBAC60E-C45E-4B51-BFDD-C2E066DFC07C}" type="presOf" srcId="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" destId="{9388E48A-AF3C-4951-A9C7-354D7C5B2D66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
+    <dgm:cxn modelId="{44758180-DB92-4090-94C7-24FEFB1C4FF3}" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" srcOrd="1" destOrd="0" parTransId="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" sibTransId="{DAE0CDDD-2988-4078-9851-07FA538106BA}"/>
+    <dgm:cxn modelId="{3254A9F3-AB89-4B45-8AF7-D6BB4771BFDC}" type="presOf" srcId="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" destId="{E7DA8D89-CCA8-4F4E-AE9E-12E48D3F5441}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{15ABE7F5-2842-4441-8A9B-B21DB4E7D6E2}" srcId="{069B2C3C-A7DF-411E-99BB-50C754EEBBA8}" destId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" srcOrd="0" destOrd="0" parTransId="{FA86B3C4-935D-4EA6-B69D-3E508927E0A4}" sibTransId="{1A6A7697-9A91-407E-94B5-6C00854098E4}"/>
+    <dgm:cxn modelId="{587FC750-A57E-41E6-9C16-F15BDFC0AB68}" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" srcOrd="0" destOrd="0" parTransId="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" sibTransId="{AF1B029C-996B-41F1-B71B-7831F8B05609}"/>
+    <dgm:cxn modelId="{61D5FC77-1C74-4BF6-B117-53E9D9FFA809}" type="presOf" srcId="{68F22967-00EF-4D13-BAEF-F5CD4D343EF6}" destId="{42E2241A-2870-46FF-8DCE-7CECD3E1329D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{5DBC543C-5BBF-454E-8905-B92A4ECF2025}" type="presOf" srcId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" destId="{578B30D0-A478-4D3A-A8E7-ECCF36290258}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{B10D13DE-BED0-4A3F-8A2A-CF05659F79FF}" srcId="{CD16E3A8-E862-4432-AB28-707CCB72B8ED}" destId="{BD914915-75E6-4220-A620-900406FDA3B2}" srcOrd="0" destOrd="0" parTransId="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" sibTransId="{51991BF6-5A78-4A79-8F43-EDD763F7EB7F}"/>
-    <dgm:cxn modelId="{ACBAC60E-C45E-4B51-BFDD-C2E066DFC07C}" type="presOf" srcId="{5855A519-8A1B-41DE-BBE9-6F57BDD401B8}" destId="{9388E48A-AF3C-4951-A9C7-354D7C5B2D66}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
-    <dgm:cxn modelId="{9BC0129D-F94A-4833-9964-064BED77EF68}" type="presOf" srcId="{069B2C3C-A7DF-411E-99BB-50C754EEBBA8}" destId="{6EB61900-881E-4E1A-A687-35C7B965E9C9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
-    <dgm:cxn modelId="{44758180-DB92-4090-94C7-24FEFB1C4FF3}" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{4188F8C2-C6B6-4BFD-82B5-BDAB6F75912E}" srcOrd="1" destOrd="0" parTransId="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" sibTransId="{DAE0CDDD-2988-4078-9851-07FA538106BA}"/>
-    <dgm:cxn modelId="{3254A9F3-AB89-4B45-8AF7-D6BB4771BFDC}" type="presOf" srcId="{B9EA2702-A89B-4AFA-AA9C-793338630C86}" destId="{E7DA8D89-CCA8-4F4E-AE9E-12E48D3F5441}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
-    <dgm:cxn modelId="{841CFBA3-9F62-4BD5-A1AC-84D8AE636CDC}" type="presOf" srcId="{17F0494C-FD27-4FD1-A051-900A836B77E6}" destId="{FAB54F49-6F1E-4DB1-AE8D-CA48304C119B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{1006F441-2900-49CA-AE4C-A89FDA5A824D}" type="presOf" srcId="{CD6CC5D0-5417-428F-AD05-1D8535E32B8E}" destId="{475D410A-9AE5-420A-8E06-1824378E493C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{3836A5FD-8F3A-4184-91AB-57736D0A77E7}" type="presParOf" srcId="{6EB61900-881E-4E1A-A687-35C7B965E9C9}" destId="{3766E119-5E72-46E5-9B3E-7281BD244EC0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
     <dgm:cxn modelId="{84A496A5-5252-471D-93EE-EC8FF72F091E}" type="presParOf" srcId="{3766E119-5E72-46E5-9B3E-7281BD244EC0}" destId="{F992707F-123D-4ADD-A0AF-9A81005FBDC8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy1"/>
@@ -5314,7 +5363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMH8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -5346,72 +5395,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="45.6" customHeight="1">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1">
       <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="111"/>
+      <c r="C2" s="113"/>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1">
       <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="111"/>
+      <c r="C3" s="113"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="114"/>
-      <c r="C4" s="114"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1">
       <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="111"/>
+      <c r="C5" s="113"/>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1">
       <c r="A6" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="110">
+      <c r="B6" s="112">
         <v>42284</v>
       </c>
-      <c r="C6" s="110"/>
+      <c r="C6" s="112"/>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1">
       <c r="A7" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="111"/>
+      <c r="C7" s="113"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="112">
+      <c r="B8" s="114">
         <v>42321</v>
       </c>
-      <c r="C8" s="113"/>
+      <c r="C8" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5433,8 +5482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -6484,10 +6533,10 @@
       <c r="AMI1"/>
     </row>
     <row r="2" spans="1:1024" ht="21.75" customHeight="1">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="114"/>
+      <c r="B2" s="116"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
@@ -7532,42 +7581,42 @@
       <c r="D4"/>
     </row>
     <row r="5" spans="1:1024" ht="19.5" customHeight="1">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="114"/>
+      <c r="B5" s="116"/>
       <c r="C5"/>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:1024" ht="42.75" customHeight="1">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="113" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="111"/>
+      <c r="B6" s="113"/>
       <c r="C6"/>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:1024" ht="21.75" customHeight="1">
-      <c r="A7" s="114" t="s">
+      <c r="A7" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="114"/>
+      <c r="B7" s="116"/>
       <c r="C7"/>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:1024" ht="146.25" customHeight="1">
-      <c r="A8" s="111" t="s">
+      <c r="A8" s="113" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="111"/>
+      <c r="B8" s="113"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:1024" ht="19.5" customHeight="1">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="114"/>
+      <c r="B9" s="116"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
@@ -7608,12 +7657,12 @@
       <c r="D13"/>
     </row>
     <row r="14" spans="1:1024" ht="20.25" customHeight="1">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
     </row>
     <row r="15" spans="1:1024" ht="27" customHeight="1" outlineLevel="1">
       <c r="A15" s="1" t="s">
@@ -7653,7 +7702,9 @@
       <c r="C17" s="109">
         <v>42325</v>
       </c>
-      <c r="D17" s="109"/>
+      <c r="D17" s="109">
+        <v>42325</v>
+      </c>
     </row>
     <row r="18" spans="1:4" outlineLevel="1">
       <c r="A18" s="3" t="s">
@@ -7665,7 +7716,9 @@
       <c r="C18" s="109">
         <v>42325</v>
       </c>
-      <c r="D18" s="83"/>
+      <c r="D18" s="109">
+        <v>42332</v>
+      </c>
     </row>
     <row r="19" spans="1:4" outlineLevel="1">
       <c r="B19" s="84"/>
@@ -7690,56 +7743,56 @@
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:4" ht="15.6" customHeight="1">
-      <c r="A23" s="114" t="s">
+      <c r="A23" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="114"/>
+      <c r="B23" s="116"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:4" ht="59.65" customHeight="1">
-      <c r="A24" s="115" t="s">
+      <c r="A24" s="117" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="115"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:4" ht="15.6" customHeight="1">
-      <c r="A25" s="114" t="s">
+      <c r="A25" s="116" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="114"/>
+      <c r="B25" s="116"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:4" ht="53.65" customHeight="1">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="117" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="115"/>
+      <c r="B26" s="117"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:4" ht="19.5" customHeight="1">
-      <c r="A27" s="114" t="s">
+      <c r="A27" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="114"/>
+      <c r="B27" s="116"/>
     </row>
     <row r="28" spans="1:4" ht="53.25" customHeight="1">
-      <c r="A28" s="115" t="s">
+      <c r="A28" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="115"/>
+      <c r="B28" s="117"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1">
-      <c r="A29" s="114" t="s">
+      <c r="A29" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="114"/>
+      <c r="B29" s="116"/>
     </row>
     <row r="30" spans="1:4" ht="45.75" customHeight="1">
-      <c r="A30" s="115" t="s">
+      <c r="A30" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="115"/>
+      <c r="B30" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -7769,7 +7822,7 @@
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -7806,13 +7859,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="15.75">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="121"/>
       <c r="F1"/>
       <c r="G1"/>
       <c r="H1"/>
@@ -13079,13 +13132,13 @@
     <row r="17" spans="1:5" outlineLevel="1"/>
     <row r="18" spans="1:5" outlineLevel="1"/>
     <row r="19" spans="1:5" outlineLevel="1">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
     </row>
     <row r="20" spans="1:5" outlineLevel="1"/>
     <row r="21" spans="1:5" outlineLevel="1"/>
@@ -13146,7 +13199,7 @@
     <row r="2" spans="1:5" ht="38.25">
       <c r="A2" s="87"/>
       <c r="B2" s="87"/>
-      <c r="C2" s="128" t="s">
+      <c r="C2" s="110" t="s">
         <v>124</v>
       </c>
       <c r="D2" s="88"/>
@@ -14319,13 +14372,13 @@
       <c r="AMI1"/>
     </row>
     <row r="2" spans="1:1024" ht="28.5" customHeight="1">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -17434,11 +17487,11 @@
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1024" s="8" customFormat="1">
-      <c r="A6" s="129"/>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024" s="8" customFormat="1">
@@ -17530,15 +17583,15 @@
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
@@ -18821,31 +18874,31 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024" s="7" customFormat="1" ht="23.25">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
       <c r="K2"/>
-      <c r="IR2" s="124" t="s">
+      <c r="IR2" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="IS2" s="124"/>
-      <c r="IT2" s="124"/>
-      <c r="IU2" s="124"/>
-      <c r="IV2" s="124"/>
-      <c r="IW2" s="124"/>
-      <c r="IX2" s="124"/>
-      <c r="IY2" s="124"/>
-      <c r="IZ2" s="124"/>
-      <c r="JA2" s="124"/>
+      <c r="IS2" s="126"/>
+      <c r="IT2" s="126"/>
+      <c r="IU2" s="126"/>
+      <c r="IV2" s="126"/>
+      <c r="IW2" s="126"/>
+      <c r="IX2" s="126"/>
+      <c r="IY2" s="126"/>
+      <c r="IZ2" s="126"/>
+      <c r="JA2" s="126"/>
     </row>
     <row r="3" spans="1:1024" s="18" customFormat="1">
       <c r="A3" s="13"/>
@@ -22331,8 +22384,8 @@
       <c r="IQ8"/>
       <c r="IR8"/>
       <c r="IS8" s="31"/>
-      <c r="IT8" s="125"/>
-      <c r="IU8" s="125"/>
+      <c r="IT8" s="127"/>
+      <c r="IU8" s="127"/>
       <c r="IV8" s="32"/>
       <c r="IW8" s="33"/>
       <c r="IX8" s="33"/>
@@ -23379,7 +23432,7 @@
       <c r="IP9"/>
       <c r="IQ9"/>
       <c r="IR9"/>
-      <c r="IS9" s="126" t="s">
+      <c r="IS9" s="128" t="s">
         <v>67</v>
       </c>
       <c r="IT9" s="35" t="s">
@@ -24431,7 +24484,7 @@
       <c r="IP10"/>
       <c r="IQ10"/>
       <c r="IR10"/>
-      <c r="IS10" s="126"/>
+      <c r="IS10" s="128"/>
       <c r="IT10" s="35" t="s">
         <v>69</v>
       </c>
@@ -25481,7 +25534,7 @@
       <c r="IP11"/>
       <c r="IQ11"/>
       <c r="IR11"/>
-      <c r="IS11" s="126"/>
+      <c r="IS11" s="128"/>
       <c r="IT11" s="35" t="s">
         <v>70</v>
       </c>
@@ -26531,7 +26584,7 @@
       <c r="IP12"/>
       <c r="IQ12"/>
       <c r="IR12"/>
-      <c r="IS12" s="126"/>
+      <c r="IS12" s="128"/>
       <c r="IT12" s="35" t="s">
         <v>71</v>
       </c>
@@ -27581,7 +27634,7 @@
       <c r="IP13"/>
       <c r="IQ13"/>
       <c r="IR13"/>
-      <c r="IS13" s="126"/>
+      <c r="IS13" s="128"/>
       <c r="IT13" s="35" t="s">
         <v>70</v>
       </c>
@@ -30716,13 +30769,13 @@
       <c r="IS16" s="59"/>
       <c r="IT16" s="60"/>
       <c r="IU16" s="36"/>
-      <c r="IV16" s="127" t="s">
+      <c r="IV16" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="IW16" s="127"/>
-      <c r="IX16" s="127"/>
-      <c r="IY16" s="127"/>
-      <c r="IZ16" s="127"/>
+      <c r="IW16" s="129"/>
+      <c r="IX16" s="129"/>
+      <c r="IY16" s="129"/>
+      <c r="IZ16" s="129"/>
       <c r="JA16"/>
       <c r="JB16"/>
       <c r="JC16"/>
@@ -33808,10 +33861,10 @@
       <c r="IP19"/>
       <c r="IQ19"/>
       <c r="IR19"/>
-      <c r="IS19" s="121" t="s">
+      <c r="IS19" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="IT19" s="121"/>
+      <c r="IT19" s="123"/>
       <c r="IU19" s="64"/>
       <c r="IV19" s="64"/>
       <c r="IW19" s="64"/>
@@ -34846,13 +34899,13 @@
       </c>
       <c r="IT20" s="67"/>
       <c r="IU20" s="64"/>
-      <c r="IV20" s="122" t="s">
+      <c r="IV20" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="IW20" s="122"/>
-      <c r="IX20" s="122"/>
-      <c r="IY20" s="122"/>
-      <c r="IZ20" s="122"/>
+      <c r="IW20" s="124"/>
+      <c r="IX20" s="124"/>
+      <c r="IY20" s="124"/>
+      <c r="IZ20" s="124"/>
       <c r="JA20"/>
       <c r="JB20"/>
       <c r="JC20"/>
@@ -35881,13 +35934,13 @@
       </c>
       <c r="IT21" s="68"/>
       <c r="IU21" s="64"/>
-      <c r="IV21" s="122" t="s">
+      <c r="IV21" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="IW21" s="122"/>
-      <c r="IX21" s="122"/>
-      <c r="IY21" s="122"/>
-      <c r="IZ21" s="122"/>
+      <c r="IW21" s="124"/>
+      <c r="IX21" s="124"/>
+      <c r="IY21" s="124"/>
+      <c r="IZ21" s="124"/>
       <c r="JA21"/>
       <c r="JB21"/>
       <c r="JC21"/>
@@ -36916,13 +36969,13 @@
       </c>
       <c r="IT22" s="69"/>
       <c r="IU22" s="64"/>
-      <c r="IV22" s="122" t="s">
+      <c r="IV22" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="IW22" s="122"/>
-      <c r="IX22" s="122"/>
-      <c r="IY22" s="122"/>
-      <c r="IZ22" s="122"/>
+      <c r="IW22" s="124"/>
+      <c r="IX22" s="124"/>
+      <c r="IY22" s="124"/>
+      <c r="IZ22" s="124"/>
       <c r="JA22"/>
       <c r="JB22"/>
       <c r="JC22"/>

</xml_diff>